<commit_message>
finish crud and filters
</commit_message>
<xml_diff>
--- a/Pokemon_Go.xlsx
+++ b/Pokemon_Go.xlsx
@@ -2992,8 +2992,8 @@
   </sheetPr>
   <dimension ref="A1:AC805"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3140,7 +3140,7 @@
         <v>90</v>
       </c>
       <c r="Q2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="3">
         <v>1</v>
@@ -3149,10 +3149,10 @@
         <v>1</v>
       </c>
       <c r="T2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="3">
         <v>5</v>
@@ -3327,7 +3327,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="2">
         <v>0</v>
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="U7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="3">
         <v>0</v>
@@ -71305,7 +71305,7 @@
         <v>0</v>
       </c>
       <c r="U801" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V801" s="3">
         <v>0</v>

</xml_diff>